<commit_message>
updated the source code to use csv traits.file
</commit_message>
<xml_diff>
--- a/files/Rubric Builder 2.5.xlsx
+++ b/files/Rubric Builder 2.5.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FOX Assessment\Fall 2020\Rubric\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asvh\Documents\GitHub\Rubrics Builder Web app\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22560" windowHeight="11290" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric Calculator Dynamic Text" sheetId="3" r:id="rId1"/>
@@ -2755,7 +2755,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:S18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="E6" sqref="E6:H6"/>
     </sheetView>
   </sheetViews>
@@ -3263,7 +3263,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E602"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>

</xml_diff>